<commit_message>
Generalize the Document class
</commit_message>
<xml_diff>
--- a/examples/InvoiceTemplate.xlsx
+++ b/examples/InvoiceTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\Documents\InvoiceGenerator\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E7542D-D672-4DE4-8A3B-9E0787D4302E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915AC7EC-0515-46FC-BAAF-48305EA57CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{0705CAA7-2CD8-4E0B-A542-4BD84EABC48A}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="3" xr2:uid="{0705CAA7-2CD8-4E0B-A542-4BD84EABC48A}"/>
   </bookViews>
   <sheets>
     <sheet name="Nomenclature" sheetId="1" r:id="rId1"/>
@@ -23,20 +23,21 @@
     <definedName name="Address" localSheetId="2">Self!$B$2</definedName>
     <definedName name="Address2" localSheetId="1">Client!$B$3</definedName>
     <definedName name="Address2" localSheetId="2">Self!$B$3</definedName>
-    <definedName name="DeliveryDate" localSheetId="3">Info!$B$5</definedName>
-    <definedName name="DocDate" localSheetId="3">Info!$B$3</definedName>
+    <definedName name="DeliveryDate" localSheetId="3">Info!$B$6</definedName>
+    <definedName name="DocDate" localSheetId="3">Info!$B$4</definedName>
     <definedName name="Mail" localSheetId="1">Client!$B$5</definedName>
     <definedName name="Mail" localSheetId="2">Self!$B$5</definedName>
     <definedName name="Name" localSheetId="1">Client!$B$1</definedName>
     <definedName name="Name" localSheetId="2">Self!$B$1</definedName>
-    <definedName name="Number" localSheetId="3">Info!$B$2</definedName>
+    <definedName name="Number" localSheetId="3">Info!$B$3</definedName>
     <definedName name="Phone" localSheetId="1">Client!$B$4</definedName>
     <definedName name="Phone" localSheetId="2">Self!$B$4</definedName>
     <definedName name="SIRET" localSheetId="1">Client!$B$6</definedName>
     <definedName name="SIRET" localSheetId="2">Self!$B$6</definedName>
-    <definedName name="StartDate" localSheetId="3">Info!$B$4</definedName>
+    <definedName name="StartDate" localSheetId="3">Info!$B$5</definedName>
+    <definedName name="Title" localSheetId="3">Info!$B$1</definedName>
     <definedName name="Total" localSheetId="0">Nomenclature!$G$2</definedName>
-    <definedName name="Type" localSheetId="3">Info!$B$1</definedName>
+    <definedName name="Type" localSheetId="3">Info!$B$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>Mail</t>
   </si>
@@ -143,6 +144,12 @@
   </si>
   <si>
     <t>Product C</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Document Title</t>
   </si>
 </sst>
 </file>
@@ -601,7 +608,7 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -829,55 +836,63 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4140B63C-002F-415A-9A60-2CE41F01486C}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="6">
-        <v>44927</v>
+        <v>16</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="6">
-        <v>44928</v>
+        <v>44927</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="6">
+        <v>44928</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B6" s="6">
         <v>44929</v>
       </c>
     </row>

</xml_diff>